<commit_message>
bi_generic_import and bi_import_chart_of_accounts added!
</commit_message>
<xml_diff>
--- a/bi_generic_import/Sample XLS-CSV File/Sample XLS File/import_picking.xlsx
+++ b/bi_generic_import/Sample XLS-CSV File/Sample XLS File/import_picking.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
   <si>
     <t xml:space="preserve">NAME</t>
   </si>
@@ -43,6 +43,24 @@
     <t xml:space="preserve">LOT</t>
   </si>
   <si>
+    <t xml:space="preserve">x_partner_id@name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x_partner_ids@name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x_color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x_notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x_amount</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x_bool</t>
+  </si>
+  <si>
     <t xml:space="preserve">WH/IN/99</t>
   </si>
   <si>
@@ -55,12 +73,21 @@
     <t xml:space="preserve">Deposit</t>
   </si>
   <si>
+    <t xml:space="preserve">Axeloer;Camptocamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red</t>
+  </si>
+  <si>
     <t xml:space="preserve">Demo</t>
   </si>
   <si>
     <t xml:space="preserve">Large Cabinet</t>
   </si>
   <si>
+    <t xml:space="preserve">blue</t>
+  </si>
+  <si>
     <t xml:space="preserve">WH/IN/25</t>
   </si>
   <si>
@@ -70,13 +97,19 @@
     <t xml:space="preserve">Pedal Bin</t>
   </si>
   <si>
+    <t xml:space="preserve">Camptocamp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">purple</t>
+  </si>
+  <si>
     <t xml:space="preserve">WH/IN/26</t>
   </si>
   <si>
-    <t xml:space="preserve">Camptocamp</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cabinet with Doors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">white</t>
   </si>
 </sst>
 </file>
@@ -88,7 +121,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="YYYY\-MM\-DD"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -109,6 +142,17 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -153,7 +197,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -162,11 +206,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -187,10 +243,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+      <selection pane="topLeft" activeCell="H6" activeCellId="0" sqref="H6:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -204,7 +260,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.37"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
@@ -226,42 +282,79 @@
       <c r="G1" s="0" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4" t="n">
         <v>42864</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>15</v>
       </c>
+      <c r="H2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="3" t="n">
+        <v>10000</v>
+      </c>
+      <c r="M2" s="6" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4" t="n">
         <v>42898</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>20</v>
@@ -269,22 +362,41 @@
       <c r="G3" s="0" t="n">
         <v>1001</v>
       </c>
+      <c r="H3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="3" t="n">
+        <v>50000</v>
+      </c>
+      <c r="M3" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="n">
+        <v>19</v>
+      </c>
+      <c r="D4" s="4" t="n">
         <v>42898</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>20</v>
@@ -292,22 +404,41 @@
       <c r="G4" s="0" t="n">
         <v>1002</v>
       </c>
+      <c r="H4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="3" t="n">
+        <v>100000</v>
+      </c>
+      <c r="M4" s="6" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="D5" s="4" t="n">
         <v>42897</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>10</v>
@@ -315,8 +446,32 @@
       <c r="G5" s="0" t="n">
         <v>1003</v>
       </c>
+      <c r="H5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="3" t="n">
+        <v>10000</v>
+      </c>
+      <c r="M5" s="6" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
     </row>
+    <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="H1" r:id="rId1" display="x_partner_id@name"/>
+    <hyperlink ref="I1" r:id="rId2" display="x_partner_ids@name"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>